<commit_message>
First persona version 2
all comments incorporated. Need better schablone. We should extract persona in pdf file.
</commit_message>
<xml_diff>
--- a/Persona_1.xlsx
+++ b/Persona_1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arinapolyanskaya/Desktop/UV/Erasmus/WebTechnologies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4236BE9-AE63-9A49-BEF6-0D371E24FCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="500" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
   </bookViews>
   <sheets>
     <sheet name="Personas Name" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -89,30 +88,6 @@
     <t>Student</t>
   </si>
   <si>
-    <t>"In order to be able to study and work, I have to know how to manage my class schedule efficently.”</t>
-  </si>
-  <si>
-    <t>Time management</t>
-  </si>
-  <si>
-    <t>Poor</t>
-  </si>
-  <si>
-    <t>Excellent</t>
-  </si>
-  <si>
-    <t>Slovak profficency</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>English profficency</t>
-  </si>
-  <si>
-    <t>Native speaker</t>
-  </si>
-  <si>
     <t>• Unclear how to include classes in the schedule</t>
   </si>
   <si>
@@ -128,49 +103,67 @@
     <t>• No idea where the courses are located on campus</t>
   </si>
   <si>
-    <t>Expereince with the website</t>
-  </si>
-  <si>
     <t>• Completing her degree successfully</t>
   </si>
   <si>
-    <t>• Reducing work-load</t>
-  </si>
-  <si>
-    <t>• Clarifying the details of her schedule</t>
-  </si>
-  <si>
-    <t>• A button for adding classes</t>
-  </si>
-  <si>
-    <t>• A button for removing classes</t>
-  </si>
-  <si>
     <t>• Identifying schedule conflicts</t>
   </si>
   <si>
-    <t>• An ability to add all classes at once</t>
-  </si>
-  <si>
-    <t>Emma is a student at the University of Bratislava studying informatics at Fyzmat. Emma usually has a busy schedule because she has a part time job and full-time university. Emma is a masters student on the third semseter. In her free time, Emma likes to do yoga, reading books and hiking.</t>
-  </si>
-  <si>
     <t>• Finding a well-paid job upon graduation</t>
   </si>
   <si>
-    <t>• Clean design easy to navigate</t>
-  </si>
-  <si>
-    <t>• Information about selected classes included</t>
-  </si>
-  <si>
     <t>• Scheduling is not connected with class registration</t>
+  </si>
+  <si>
+    <t>Emma is a student at the University in Bratislava. Emma usually has a busy schedule because she has a part time job and full-time university. Emma is a masters student on the third semseter. In her free time, Emma likes to do yoga, reading books and hiking.</t>
+  </si>
+  <si>
+    <t>• Possibility add to schedule nonschool activities</t>
+  </si>
+  <si>
+    <t>• Clarifying the details of her school subjects</t>
+  </si>
+  <si>
+    <t>• Better knowledge about her study program and class placement</t>
+  </si>
+  <si>
+    <t>• search class, registrate and add it</t>
+  </si>
+  <si>
+    <t>• remove class I want (in correct datum)</t>
+  </si>
+  <si>
+    <t>• An ability to add, registarte in all classes at once</t>
+  </si>
+  <si>
+    <t>• Details of class contain your marks and materials</t>
+  </si>
+  <si>
+    <t>•Information which study program I have choosed and graduation year</t>
+  </si>
+  <si>
+    <t>•Show schedule only when I am logged in</t>
+  </si>
+  <si>
+    <t>Mobile vs PC</t>
+  </si>
+  <si>
+    <t>Slovak vs English profficency</t>
+  </si>
+  <si>
+    <t>Every clasification in details or all clasifications independent</t>
+  </si>
+  <si>
+    <t>"In order to be able to study and work, I have to know how to manage my class schedule efficently with my work schedule.”</t>
+  </si>
+  <si>
+    <t>Schedule vs timetable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -324,12 +317,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -346,9 +340,17 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,18 +360,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -407,7 +400,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5302250" y="1880943"/>
+          <a:off x="4901946" y="1864687"/>
           <a:ext cx="2009775" cy="102381"/>
           <a:chOff x="158" y="0"/>
           <a:chExt cx="1999991" cy="91005"/>
@@ -603,7 +596,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5285122" y="2117048"/>
+          <a:off x="4884818" y="2098760"/>
           <a:ext cx="2009775" cy="99631"/>
           <a:chOff x="48" y="0"/>
           <a:chExt cx="2000281" cy="88561"/>
@@ -799,7 +792,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7406005" y="1854835"/>
+          <a:off x="8995029" y="1840611"/>
           <a:ext cx="2059935" cy="98218"/>
           <a:chOff x="4" y="0"/>
           <a:chExt cx="2050356" cy="87304"/>
@@ -995,7 +988,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7390765" y="2101215"/>
+          <a:off x="8987409" y="2079879"/>
           <a:ext cx="2019300" cy="85725"/>
           <a:chOff x="26" y="0"/>
           <a:chExt cx="2009836" cy="76200"/>
@@ -1513,411 +1506,388 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="13.83203125" customWidth="1"/>
+    <col min="1" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="5" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+    <col min="7" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="37.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18"/>
-      <c r="B1" s="11"/>
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="20" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="18">
         <v>23</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="14" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="16"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="13" t="s">
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="16"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="10" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="16"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-    </row>
-    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-    </row>
-    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+        <v>34</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -1937,28 +1907,37 @@
       <c r="I26" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="55">
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="A8:E11"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="F11:G11"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A1:B5"/>
@@ -1968,16 +1947,11 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:I5"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="G18:I18"/>
@@ -1989,9 +1963,6 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>